<commit_message>
Inertia and f_decay don't work
</commit_message>
<xml_diff>
--- a/DE_Tests.xlsx
+++ b/DE_Tests.xlsx
@@ -1,68 +1,18 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
-  </bookViews>
-  <sheets>
-    <sheet name="population_size" r:id="rId1" sheetId="1"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
-</workbook>
-</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>population_size = 30</t>
-  </si>
-  <si>
-    <t>Dimensions</t>
-  </si>
-  <si>
-    <t>population_size = 10</t>
-  </si>
-  <si>
-    <t>rozenbrock</t>
-  </si>
-  <si>
-    <t>Success Ratio</t>
-  </si>
-  <si>
-    <t>population_size = 100</t>
-  </si>
-  <si>
-    <t>Function Evals</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,12 +35,8 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -381,107 +327,4 @@
   <ns0:objectDefaults/>
   <ns0:extraClrSchemeLst/>
 </ns0:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
-  </sheetPr>
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col max="1" collapsed="0" customWidth="true" width="15" min="1"/>
-    <col max="3" collapsed="0" customWidth="true" width="15" min="3"/>
-    <col max="2" collapsed="0" customWidth="true" width="15" min="2"/>
-    <col max="5" collapsed="0" customWidth="true" width="15" min="5"/>
-    <col max="4" collapsed="0" customWidth="true" width="15" min="4"/>
-    <col max="7" collapsed="0" customWidth="true" width="15" min="7"/>
-    <col max="6" collapsed="0" customWidth="true" width="15" min="6"/>
-    <col max="9" collapsed="0" width="9.10" min="9"/>
-    <col max="8" collapsed="0" customWidth="true" width="15" min="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c s="1" r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c s="1" r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c s="2" r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c s="1" r="D1" t="s"/>
-      <c s="2" r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c s="1" r="F1" t="s"/>
-      <c s="2" r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c s="1" r="H1" t="s"/>
-      <c s="1" r="I1" t="s"/>
-    </row>
-    <row r="2" spans="1:9">
-      <c s="1" r="A2" t="s"/>
-      <c s="1" r="B2" t="s"/>
-      <c s="1" r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c s="1" r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c s="1" r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c s="1" r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c s="1" r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c s="1" r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c s="1" r="I2" t="s"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.20000000000000001</v>
-      </c>
-      <c r="D3" t="n">
-        <v>8410.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>11070.0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>21200.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-  </mergeCells>
-</worksheet>
 </file>
</xml_diff>